<commit_message>
adding overview, essential commit history
</commit_message>
<xml_diff>
--- a/commit_history/noteblock_frontend_commit_and_issue_history.xlsx
+++ b/commit_history/noteblock_frontend_commit_and_issue_history.xlsx
@@ -8,17 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NoteBlock\doc_repos\NoteBlockWorkHistory\commit_history\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A696B6DD-5508-489D-8555-05EED81458CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60EF2DED-E292-4510-B999-DF10460C18D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="-192" windowWidth="23232" windowHeight="12696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="5" r:id="rId1"/>
     <sheet name="Commit_history_1stRepo" sheetId="1" r:id="rId2"/>
-    <sheet name="Commit_history_forkedRepoPROD" sheetId="2" r:id="rId3"/>
+    <sheet name="Commit_history_forkedRepoPROD" sheetId="6" r:id="rId3"/>
     <sheet name="Issue_history_1stRepo" sheetId="3" r:id="rId4"/>
     <sheet name="Issue_history_forkedRepoPROD" sheetId="4" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="tblFirstRepoCommit" localSheetId="2">Table14[#All]</definedName>
+    <definedName name="tblFirstRepoCommit">Table1[#All]</definedName>
+    <definedName name="tblFirstRepoCommitHistory" localSheetId="2">Table14[#All]</definedName>
+    <definedName name="tblFirstRepoCommitHistory">Table1[#All]</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -29,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="42">
   <si>
     <t>Branch</t>
   </si>
@@ -83,13 +89,162 @@
   </si>
   <si>
     <t>Branch in Antony's forked repo</t>
+  </si>
+  <si>
+    <t>Commit Hash</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>sso-auth</t>
+  </si>
+  <si>
+    <t>sso-auth-ts</t>
+  </si>
+  <si>
+    <t>Mark</t>
+  </si>
+  <si>
+    <t>Antony</t>
+  </si>
+  <si>
+    <r>
+      <t>4343be788497cdbc47776eb79fd712cf0fde16fe</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="5"/>
+        <color rgb="FF24292F"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>f339ba30a048ff9596e3cafd2802da34e4bb7448</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="5"/>
+        <color rgb="FF24292F"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>bc91a87a5a8e1babef0d401207c6026b5db36604</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="5"/>
+        <color rgb="FF24292F"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1f70c1df4cae0556387687445abfc7483394b8a2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="5"/>
+        <color rgb="FF24292F"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>42ae855af652ff9e343154c98f57719766ea38df</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="5"/>
+        <color rgb="FF24292F"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <t>Init commit</t>
+  </si>
+  <si>
+    <t>Adding AuthProvider</t>
+  </si>
+  <si>
+    <t>Adding Auth to existing Sign Up button</t>
+  </si>
+  <si>
+    <t>README.md update to describe changes</t>
+  </si>
+  <si>
+    <t>Upgrades to enable typescript in app for future development</t>
+  </si>
+  <si>
+    <r>
+      <t>e7867a44a656497ad2e135de1532283f3fac5add</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="5"/>
+        <color rgb="FF24292F"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <t>Antony Forked Repo: tonylulciuc:typescript-upgrade</t>
+  </si>
+  <si>
+    <t>Adding typescript v 4.4.3 to package.json + tsconfig where include is applied to all files in src + test upgrades</t>
+  </si>
+  <si>
+    <r>
+      <t>0eaf1e32faf19a145151a5c9101b68c7971ec24c</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="5"/>
+        <color rgb="FF24292F"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <t>Minor .gitignore updates</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Mark forking from private repo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,6 +268,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="5"/>
+      <color rgb="FF24292F"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -134,7 +295,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -147,11 +308,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -162,6 +333,32 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A7F47AE2-078E-4FF9-A36C-C274082B4549}" name="Table1" displayName="Table1" ref="B2:E7" totalsRowShown="0">
+  <autoFilter ref="B2:E7" xr:uid="{A7F47AE2-078E-4FF9-A36C-C274082B4549}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{6EC53481-1EDE-4DC2-A78D-34C4F0CC31C7}" name="Branch"/>
+    <tableColumn id="2" xr3:uid="{4842BE9E-83D4-467C-8037-A556551382DC}" name="Commit Hash"/>
+    <tableColumn id="3" xr3:uid="{6591D0E0-C173-4269-82F1-DD152246D738}" name="User"/>
+    <tableColumn id="4" xr3:uid="{FE86B28A-6A47-4D59-BBEB-3E276EF33DBB}" name="Description" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0CBB60CF-A237-4BF9-94B3-4E2BC1E4ECE2}" name="Table14" displayName="Table14" ref="B2:E5" totalsRowShown="0">
+  <autoFilter ref="B2:E5" xr:uid="{A7F47AE2-078E-4FF9-A36C-C274082B4549}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{02128AC8-9353-455A-8814-05E7E335A171}" name="Branch"/>
+    <tableColumn id="2" xr3:uid="{D93A1315-6DF6-45AA-A22D-9A3EF5960C8D}" name="Commit Hash"/>
+    <tableColumn id="3" xr3:uid="{E414130F-894F-4508-8A8D-C0E81AC4FA91}" name="User"/>
+    <tableColumn id="4" xr3:uid="{432AB361-38DA-4908-B6B0-041626A9CF08}" name="Description" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -430,7 +627,7 @@
   <dimension ref="B3:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -628,36 +825,189 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2"/>
+  <dimension ref="B2:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="15.7890625" customWidth="1"/>
+    <col min="2" max="2" width="16.20703125" customWidth="1"/>
+    <col min="3" max="3" width="41.83984375" customWidth="1"/>
+    <col min="4" max="4" width="12.734375" customWidth="1"/>
+    <col min="5" max="5" width="64.15625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B2" t="s">
         <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7716EF20-3A72-424A-8BC5-C5F56EC05DCD}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9622785-481D-461A-AB16-3E24998440B6}">
+  <dimension ref="B2:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="25.20703125" customWidth="1"/>
+    <col min="3" max="3" width="41.83984375" customWidth="1"/>
+    <col min="4" max="4" width="12.734375" customWidth="1"/>
+    <col min="5" max="5" width="64.15625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B4" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B5" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>